<commit_message>
Adding new experiment, modifying old one
</commit_message>
<xml_diff>
--- a/data/expulsion_processed_2016_11_23.xlsx
+++ b/data/expulsion_processed_2016_11_23.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denise\Documents\Mandel Lab\Assays - Squid Comps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denise\Documents\coding\data_visualization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="graph" sheetId="3" r:id="rId3"/>
     <sheet name="python" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="35">
   <si>
     <t>colonizer</t>
   </si>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -401,6 +401,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADB1-4D12-8F48-BE0CD8365848}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -537,6 +542,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ADB1-4D12-8F48-BE0CD8365848}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -623,6 +633,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-ADB1-4D12-8F48-BE0CD8365848}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -932,7 +947,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1146,6 +1161,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A199-4451-B1A4-85D2C2641B63}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1282,6 +1302,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A199-4451-B1A4-85D2C2641B63}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1368,6 +1393,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A199-4451-B1A4-85D2C2641B63}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1677,7 +1707,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1892,6 +1922,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-98A4-4BB7-AF62-4B73263241DE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2035,6 +2070,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-98A4-4BB7-AF62-4B73263241DE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2121,6 +2161,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-98A4-4BB7-AF62-4B73263241DE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2430,7 +2475,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2645,6 +2690,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-035C-4E71-9556-08EEECE061AE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2781,6 +2831,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-035C-4E71-9556-08EEECE061AE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2867,6 +2922,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-035C-4E71-9556-08EEECE061AE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5606,6 +5666,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5641,6 +5718,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10217,7 +10311,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10289,8 +10383,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>3</v>
+      <c r="A7">
+        <v>11</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -10300,8 +10394,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>3</v>
+      <c r="A8">
+        <v>11</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -10311,8 +10405,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>3</v>
+      <c r="A9">
+        <v>11</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -10322,8 +10416,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>3</v>
+      <c r="A10">
+        <v>11</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -10333,8 +10427,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>3</v>
+      <c r="A11">
+        <v>11</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -10344,8 +10438,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>3</v>
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12">
         <v>12</v>
@@ -10355,8 +10449,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>4</v>
+      <c r="A13">
+        <v>22</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -10366,8 +10460,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>4</v>
+      <c r="A14">
+        <v>22</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -10377,8 +10471,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>4</v>
+      <c r="A15">
+        <v>22</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -10388,8 +10482,8 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>4</v>
+      <c r="A16">
+        <v>22</v>
       </c>
       <c r="B16">
         <v>8</v>
@@ -10399,8 +10493,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>4</v>
+      <c r="A17">
+        <v>22</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -10410,8 +10504,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>4</v>
+      <c r="A18">
+        <v>22</v>
       </c>
       <c r="B18">
         <v>12</v>

</xml_diff>